<commit_message>
button function for get_dash
</commit_message>
<xml_diff>
--- a/get_dash/expense.xlsx
+++ b/get_dash/expense.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
   <si>
     <t>type</t>
   </si>
@@ -46,6 +46,9 @@
   <si>
     <t>other</t>
   </si>
+  <si>
+    <t>study</t>
+  </si>
 </sst>
 </file>
 
@@ -54,8 +57,8 @@
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd\ h:mm:ss"/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -67,6 +70,72 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -76,61 +145,26 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -150,14 +184,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -176,29 +202,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -220,19 +223,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -244,91 +385,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -340,67 +397,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,30 +414,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -453,37 +432,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,16 +460,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -529,133 +532,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1019,7 +1022,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1130,7 +1133,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C8" s="3">
         <v>44438</v>
@@ -1155,10 +1158,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B10" s="1">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="C10" s="3">
         <v>44438</v>

</xml_diff>

<commit_message>
fix some bug in get_dash
</commit_message>
<xml_diff>
--- a/get_dash/expense.xlsx
+++ b/get_dash/expense.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,20 +441,35 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Unnamed: 0.1.1.1</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>amount</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>userId</t>
         </is>
@@ -467,20 +482,29 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="G2" t="n">
         <v>10</v>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>2021-08-29</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -493,20 +517,29 @@
       <c r="B3" t="n">
         <v>1</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>clothing</t>
-        </is>
+      <c r="C3" t="n">
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" t="inlineStr">
         <is>
           <t>2021-07-26</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>Dixon3221</t>
         </is>
@@ -519,20 +552,29 @@
       <c r="B4" t="n">
         <v>2</v>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F4" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="D4" t="n">
-        <v>3</v>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="G4" t="n">
+        <v>20</v>
+      </c>
+      <c r="H4" t="inlineStr">
         <is>
           <t>2021-06-14</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -545,20 +587,29 @@
       <c r="B5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>transportation</t>
-        </is>
+      <c r="C5" t="n">
+        <v>3</v>
       </c>
       <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>entertain</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
         <v>80</v>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>2021-08-20</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -571,20 +622,29 @@
       <c r="B6" t="n">
         <v>4</v>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="D6" t="n">
+      <c r="G6" t="n">
         <v>422</v>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>2021-06-14</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -597,20 +657,29 @@
       <c r="B7" t="n">
         <v>5</v>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>5</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="D7" t="n">
-        <v>68.7</v>
-      </c>
-      <c r="E7" t="inlineStr">
+      <c r="G7" t="n">
+        <v>60.9</v>
+      </c>
+      <c r="H7" t="inlineStr">
         <is>
           <t>2021-08-21</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -621,22 +690,31 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr">
+        <v>6</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" t="n">
+        <v>6</v>
+      </c>
+      <c r="E8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="G8" t="n">
         <v>20</v>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -647,22 +725,31 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr">
+        <v>7</v>
+      </c>
+      <c r="C9" t="n">
+        <v>7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7</v>
+      </c>
+      <c r="F9" t="inlineStr">
         <is>
           <t>study</t>
         </is>
       </c>
-      <c r="D9" t="n">
+      <c r="G9" t="n">
         <v>20</v>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -673,22 +760,31 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr">
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8</v>
+      </c>
+      <c r="D10" t="n">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F10" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="G10" t="n">
         <v>4.8</v>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -698,21 +794,32 @@
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr">
+      <c r="B11" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>9</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9</v>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>others</t>
         </is>
       </c>
-      <c r="D11" t="n">
+      <c r="G11" t="n">
         <v>20</v>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -722,21 +829,296 @@
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>entertainment</t>
-        </is>
+      <c r="B12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10</v>
       </c>
       <c r="D12" t="n">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="G12" t="n">
+        <v>40</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>2021-08-30</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>11</v>
+      </c>
+      <c r="C13" t="n">
+        <v>11</v>
+      </c>
+      <c r="D13" t="n">
+        <v>11</v>
+      </c>
+      <c r="E13" t="n">
+        <v>11</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>food</t>
+        </is>
+      </c>
+      <c r="G13" t="n">
+        <v>40</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>2021-08-30</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>12</v>
+      </c>
+      <c r="C14" t="n">
+        <v>12</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="n">
+        <v>12</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
+      <c r="G14" t="n">
+        <v>20</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2021-08-30</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>13</v>
+      </c>
+      <c r="C15" t="n">
+        <v>13</v>
+      </c>
+      <c r="D15" t="n">
+        <v>13</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="G15" t="n">
         <v>30</v>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>2021-08-30</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2021-09-01</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>14</v>
+      </c>
+      <c r="C16" t="n">
+        <v>14</v>
+      </c>
+      <c r="D16" t="n">
+        <v>14</v>
+      </c>
+      <c r="E16" t="n">
+        <v>14</v>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>transport</t>
+        </is>
+      </c>
+      <c r="G16" t="n">
+        <v>300</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2021-09-03</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>15</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15</v>
+      </c>
+      <c r="D17" t="n">
+        <v>15</v>
+      </c>
+      <c r="E17" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="G17" t="n">
+        <v>40</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2021-08-31</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>16</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16</v>
+      </c>
+      <c r="D18" t="n">
+        <v>16</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>entertain</t>
+        </is>
+      </c>
+      <c r="G18" t="n">
+        <v>25</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2021-09-01</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>17</v>
+      </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>study</t>
+        </is>
+      </c>
+      <c r="G19" t="n">
+        <v>26</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>2021-09-02</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
+      <c r="E20" t="inlineStr"/>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="G20" t="n">
+        <v>10</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>2021-09-02</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>

</xml_diff>

<commit_message>
fix bugs in get_dash
</commit_message>
<xml_diff>
--- a/get_dash/expense.xlsx
+++ b/get_dash/expense.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,20 +456,25 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>Unnamed: 0.1.1.1.1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>type</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>amount</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>date</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>userId</t>
         </is>
@@ -491,20 +496,23 @@
       <c r="E2" t="n">
         <v>0</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>10</v>
       </c>
-      <c r="H2" t="inlineStr">
+      <c r="I2" t="inlineStr">
         <is>
           <t>2021-08-29</t>
         </is>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -526,20 +534,23 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>2021-07-26</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Dixon3221</t>
         </is>
@@ -561,20 +572,23 @@
       <c r="E4" t="n">
         <v>2</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>20</v>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I4" t="inlineStr">
         <is>
           <t>2021-06-14</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -596,20 +610,23 @@
       <c r="E5" t="n">
         <v>3</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>entertain</t>
         </is>
       </c>
-      <c r="G5" t="n">
-        <v>80</v>
-      </c>
-      <c r="H5" t="inlineStr">
+      <c r="H5" t="n">
+        <v>70</v>
+      </c>
+      <c r="I5" t="inlineStr">
         <is>
           <t>2021-08-20</t>
         </is>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -631,20 +648,23 @@
       <c r="E6" t="n">
         <v>4</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>other</t>
         </is>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>422</v>
       </c>
-      <c r="H6" t="inlineStr">
+      <c r="I6" t="inlineStr">
         <is>
           <t>2021-06-14</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -666,20 +686,23 @@
       <c r="E7" t="n">
         <v>5</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>5</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>60.9</v>
       </c>
-      <c r="H7" t="inlineStr">
+      <c r="I7" t="inlineStr">
         <is>
           <t>2021-08-21</t>
         </is>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -701,20 +724,23 @@
       <c r="E8" t="n">
         <v>6</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>6</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>20</v>
       </c>
-      <c r="H8" t="inlineStr">
+      <c r="I8" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -736,20 +762,23 @@
       <c r="E9" t="n">
         <v>7</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>7</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>study</t>
         </is>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>20</v>
       </c>
-      <c r="H9" t="inlineStr">
+      <c r="I9" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -771,20 +800,23 @@
       <c r="E10" t="n">
         <v>8</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="n">
+        <v>8</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>4.8</v>
       </c>
-      <c r="H10" t="inlineStr">
+      <c r="I10" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -806,20 +838,23 @@
       <c r="E11" t="n">
         <v>9</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="n">
+        <v>9</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>others</t>
         </is>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>20</v>
       </c>
-      <c r="H11" t="inlineStr">
+      <c r="I11" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -841,20 +876,23 @@
       <c r="E12" t="n">
         <v>10</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>10</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>40</v>
       </c>
-      <c r="H12" t="inlineStr">
+      <c r="I12" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -876,20 +914,23 @@
       <c r="E13" t="n">
         <v>11</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="n">
+        <v>11</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>food</t>
         </is>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>40</v>
       </c>
-      <c r="H13" t="inlineStr">
+      <c r="I13" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -911,20 +952,23 @@
       <c r="E14" t="n">
         <v>12</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="n">
+        <v>12</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>others</t>
         </is>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>20</v>
       </c>
-      <c r="H14" t="inlineStr">
+      <c r="I14" t="inlineStr">
         <is>
           <t>2021-08-30</t>
         </is>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -946,20 +990,23 @@
       <c r="E15" t="n">
         <v>13</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="n">
+        <v>13</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>30</v>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="I15" t="inlineStr">
         <is>
           <t>2021-09-01</t>
         </is>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -981,20 +1028,23 @@
       <c r="E16" t="n">
         <v>14</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>14</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>transport</t>
         </is>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>300</v>
       </c>
-      <c r="H16" t="inlineStr">
+      <c r="I16" t="inlineStr">
         <is>
           <t>2021-09-03</t>
         </is>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -1016,20 +1066,23 @@
       <c r="E17" t="n">
         <v>15</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="n">
+        <v>15</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>40</v>
       </c>
-      <c r="H17" t="inlineStr">
+      <c r="I17" t="inlineStr">
         <is>
           <t>2021-08-31</t>
         </is>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -1048,21 +1101,24 @@
       <c r="D18" t="n">
         <v>16</v>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr">
+      <c r="E18" t="n">
+        <v>16</v>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
         <is>
           <t>entertain</t>
         </is>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>25</v>
       </c>
-      <c r="H18" t="inlineStr">
+      <c r="I18" t="inlineStr">
         <is>
           <t>2021-09-01</t>
         </is>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -1075,23 +1131,26 @@
       <c r="B19" t="n">
         <v>17</v>
       </c>
-      <c r="C19" t="inlineStr"/>
+      <c r="C19" t="n">
+        <v>17</v>
+      </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
         <is>
           <t>study</t>
         </is>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>26</v>
       </c>
-      <c r="H19" t="inlineStr">
+      <c r="I19" t="inlineStr">
         <is>
           <t>2021-09-02</t>
         </is>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>
@@ -1101,24 +1160,55 @@
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>18</v>
+      </c>
       <c r="C20" t="inlineStr"/>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
         <is>
           <t>clothing</t>
         </is>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>10</v>
       </c>
-      <c r="H20" t="inlineStr">
+      <c r="I20" t="inlineStr">
         <is>
           <t>2021-09-02</t>
         </is>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Dixon3220</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>clothing</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>40</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2021-08-20</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
         <is>
           <t>Dixon3220</t>
         </is>

</xml_diff>